<commit_message>
added spaces before sub articles in md
</commit_message>
<xml_diff>
--- a/styles/styles.xlsx
+++ b/styles/styles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://flexup0.sharepoint.com/sites/FlexUpSharedFolder/Shared Documents/Legal/Styles/styles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="143" documentId="8_{B03146FB-B39C-4187-A8DA-49626FBC9375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B53D1FF-8D6B-43E9-88F5-14E0CEF30E31}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="8_{B03146FB-B39C-4187-A8DA-49626FBC9375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02ABAA05-7FAE-4A89-BBDE-B58ACFFB5BD9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6AF5B7A2-C91E-4868-8B5D-CDD1E4182A17}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{6AF5B7A2-C91E-4868-8B5D-CDD1E4182A17}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="100">
   <si>
     <t>FlexUp Word - Mardown Style Guidelines</t>
   </si>
@@ -296,9 +296,6 @@
     <t>## Section A. &lt;text&gt;</t>
   </si>
   <si>
-    <t>### 1. &lt;text&gt;</t>
-  </si>
-  <si>
     <t>[^label]: &lt;text&gt;</t>
   </si>
   <si>
@@ -333,6 +330,12 @@
   </si>
   <si>
     <t>6</t>
+  </si>
+  <si>
+    <t>1. &lt;text&gt;</t>
+  </si>
+  <si>
+    <t>12</t>
   </si>
 </sst>
 </file>
@@ -786,32 +789,32 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="16" defaultRowHeight="15" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="2" width="16" style="1"/>
-    <col min="3" max="3" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="1" customWidth="1"/>
-    <col min="10" max="14" width="11.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.3046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.3046875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.84375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.15234375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.15234375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.53515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.15234375" style="1" customWidth="1"/>
+    <col min="10" max="14" width="11.3046875" style="2" customWidth="1"/>
     <col min="15" max="16384" width="16" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" ht="20.6" x14ac:dyDescent="0.65">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="7" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="7" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="8" t="s">
         <v>55</v>
       </c>
@@ -855,7 +858,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>56</v>
       </c>
@@ -889,7 +892,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>57</v>
       </c>
@@ -925,7 +928,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>58</v>
       </c>
@@ -961,7 +964,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>59</v>
       </c>
@@ -995,7 +998,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1011,13 +1014,13 @@
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
     </row>
-    <row r="9" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>16</v>
@@ -1037,13 +1040,13 @@
       </c>
       <c r="N9" s="4"/>
     </row>
-    <row r="10" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>16</v>
@@ -1056,7 +1059,7 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M10" s="4">
         <v>6</v>
@@ -1065,7 +1068,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>70</v>
       </c>
@@ -1073,7 +1076,7 @@
         <v>39</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>16</v>
@@ -1093,7 +1096,7 @@
       </c>
       <c r="N11" s="4"/>
     </row>
-    <row r="12" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
         <v>71</v>
       </c>
@@ -1101,7 +1104,7 @@
         <v>73</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>16</v>
@@ -1121,7 +1124,7 @@
       </c>
       <c r="N12" s="4"/>
     </row>
-    <row r="13" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
         <v>72</v>
       </c>
@@ -1129,7 +1132,7 @@
         <v>74</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>16</v>
@@ -1149,7 +1152,7 @@
       </c>
       <c r="N13" s="4"/>
     </row>
-    <row r="14" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1165,7 +1168,7 @@
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
     </row>
-    <row r="15" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
         <v>60</v>
       </c>
@@ -1205,7 +1208,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
         <v>10</v>
       </c>
@@ -1247,7 +1250,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
         <v>11</v>
       </c>
@@ -1289,7 +1292,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
         <v>12</v>
       </c>
@@ -1297,7 +1300,7 @@
         <v>15</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>16</v>
@@ -1331,7 +1334,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
         <v>61</v>
       </c>
@@ -1339,7 +1342,7 @@
         <v>15</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>16</v>
@@ -1373,7 +1376,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1389,7 +1392,7 @@
       <c r="M20" s="4"/>
       <c r="N20" s="5"/>
     </row>
-    <row r="21" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A21" s="4" t="s">
         <v>62</v>
       </c>
@@ -1423,7 +1426,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A22" s="4" t="s">
         <v>63</v>
       </c>
@@ -1457,7 +1460,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1473,7 +1476,7 @@
       <c r="M23" s="4"/>
       <c r="N23" s="5"/>
     </row>
-    <row r="24" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
         <v>64</v>
       </c>
@@ -1513,7 +1516,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A25" s="4" t="s">
         <v>65</v>
       </c>
@@ -1555,7 +1558,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A26" s="4" t="s">
         <v>34</v>
       </c>
@@ -1563,14 +1566,14 @@
         <v>5</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>32</v>
@@ -1585,8 +1588,8 @@
       <c r="K26" s="5">
         <v>0.75</v>
       </c>
-      <c r="L26" s="4">
-        <v>18</v>
+      <c r="L26" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="M26" s="4">
         <v>6</v>
@@ -1595,7 +1598,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="4" t="s">
         <v>36</v>
       </c>
@@ -1603,7 +1606,7 @@
         <v>15</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>16</v>
@@ -1637,7 +1640,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A28" s="4" t="s">
         <v>66</v>
       </c>
@@ -1645,7 +1648,7 @@
         <v>15</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>16</v>
@@ -1679,7 +1682,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1695,7 +1698,7 @@
       <c r="M29" s="4"/>
       <c r="N29" s="5"/>
     </row>
-    <row r="30" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="4" t="s">
         <v>67</v>
       </c>
@@ -1729,7 +1732,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="4" t="s">
         <v>68</v>
       </c>
@@ -1737,7 +1740,7 @@
         <v>53</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>54</v>
@@ -1763,7 +1766,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A32" s="4" t="s">
         <v>69</v>
       </c>
@@ -1771,7 +1774,7 @@
         <v>53</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>16</v>
@@ -1804,6 +1807,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="585e1850-a672-4c59-9766-e6f9b47acd25" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c94c4ac8-faf4-477a-b4e6-6adaeda6e30a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D6773F011C44794EBD166792D78297B2" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3820cfa27876710366705819bfadb0e3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c94c4ac8-faf4-477a-b4e6-6adaeda6e30a" xmlns:ns3="585e1850-a672-4c59-9766-e6f9b47acd25" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="499fff40122d1a2e24091cbf6e45c141" ns2:_="" ns3:_="">
     <xsd:import namespace="c94c4ac8-faf4-477a-b4e6-6adaeda6e30a"/>
@@ -1998,27 +2021,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="585e1850-a672-4c59-9766-e6f9b47acd25" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c94c4ac8-faf4-477a-b4e6-6adaeda6e30a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C9A5F7-7B5B-407C-8EEF-0A1EF343B4EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{331E6862-8E9F-4011-AD50-43EF39F1C7AA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="585e1850-a672-4c59-9766-e6f9b47acd25"/>
+    <ds:schemaRef ds:uri="c94c4ac8-faf4-477a-b4e6-6adaeda6e30a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A27EA518-EDA4-46D8-B000-A7D6AF3AFAC2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2035,23 +2057,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{331E6862-8E9F-4011-AD50-43EF39F1C7AA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="585e1850-a672-4c59-9766-e6f9b47acd25"/>
-    <ds:schemaRef ds:uri="c94c4ac8-faf4-477a-b4e6-6adaeda6e30a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83C9A5F7-7B5B-407C-8EEF-0A1EF343B4EB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>